<commit_message>
still trying to get random testimonials to render
</commit_message>
<xml_diff>
--- a/db/malas-data-20220207.xlsx
+++ b/db/malas-data-20220207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morganb/Development/code/Mod5/morgan-moonchild/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B062A0B8-C973-074E-9F15-2A50D4C5C30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158C344F-113E-D44A-9827-8C280853B2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="1380" windowWidth="32060" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="660" windowWidth="32060" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - EtsyListingsDownload-" sheetId="1" r:id="rId1"/>
@@ -4668,11 +4668,11 @@
   </sheetPr>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="117.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="166.6640625" style="1" customWidth="1"/>
@@ -4681,10 +4681,10 @@
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="6" width="158.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="108.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="69.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="69.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="69.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="69.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="44" style="1" customWidth="1"/>
     <col min="12" max="12" width="69.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="69.83203125" style="1" customWidth="1"/>
     <col min="14" max="15" width="69.6640625" style="1" customWidth="1"/>
@@ -4693,7 +4693,7 @@
     <col min="20" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
         <v>356</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="152.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="176" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="176" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="128" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>44</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="128" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>59</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="104" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>74</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="164" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>89</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="260" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>103</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="152" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>117</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="140" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>132</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="128" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>137</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="140" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>150</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="152" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>165</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="188" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>180</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="116" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>194</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="284" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>209</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="128" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>223</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="104" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>237</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="248" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>252</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="152" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>267</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="176" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>282</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="212" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>297</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="296" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
         <v>311</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="164" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>325</v>
       </c>

</xml_diff>